<commit_message>
sensactHsNano for Reflow Soldering
</commit_message>
<xml_diff>
--- a/pcb/sensactHsNano/PinHints.xlsx
+++ b/pcb/sensactHsNano/PinHints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\ESP32DeviceController\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\sensact\pcb\sensactHsNano\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5FFAEC-92C4-4FBD-A6CA-5BFD3BBE35A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F69A2B2-234B-4AB0-BC0D-D2D73050E215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2190" yWindow="2055" windowWidth="21600" windowHeight="11385" xr2:uid="{CF3DADBF-83E5-4D16-A608-914491EF0B5B}"/>
+    <workbookView xWindow="29970" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{CF3DADBF-83E5-4D16-A608-914491EF0B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>GPIO</t>
   </si>
@@ -120,39 +120,9 @@
     <t>ModulePin</t>
   </si>
   <si>
-    <t>sensactIO4</t>
-  </si>
-  <si>
-    <t>Muss TX bleiben</t>
-  </si>
-  <si>
     <t>Ist natürlich zunächst RX, also Input. Könnte aber umgestellt werden</t>
   </si>
   <si>
-    <t>I2C_SDA</t>
-  </si>
-  <si>
-    <t>I2C_SCL</t>
-  </si>
-  <si>
-    <t>I12</t>
-  </si>
-  <si>
-    <t>I13</t>
-  </si>
-  <si>
-    <t>I14</t>
-  </si>
-  <si>
-    <t>O13</t>
-  </si>
-  <si>
-    <t>I15</t>
-  </si>
-  <si>
-    <t>O14</t>
-  </si>
-  <si>
     <t>STRAPPING: If driven High, flash voltage (VDD_SDIO) is 1.8V not default 3.3V.</t>
   </si>
   <si>
@@ -168,13 +138,7 @@
     <t>STRAPPING: Irgendwelche Tining-Eigenschaften des SDIO einstellen</t>
   </si>
   <si>
-    <t>O15</t>
-  </si>
-  <si>
-    <t>O12 mit Jumper --&gt;macht nichts, wenn "silent"…und bei Bedarf mit Jumper verändern</t>
-  </si>
-  <si>
-    <t>Pull-Low-Switch+LED</t>
+    <t>sensactHsNano</t>
   </si>
 </sst>
 </file>
@@ -257,7 +221,7 @@
     <tableColumn id="3" xr3:uid="{940DC012-9DCD-475A-A479-DCB44590E186}" name="Eigenschaft"/>
     <tableColumn id="4" xr3:uid="{ACE45FE6-304F-49D6-87E9-A0A0579929EC}" name="Folgerung"/>
     <tableColumn id="5" xr3:uid="{FFC6BE79-3EAC-423D-B26D-726E0897F39B}" name="Beschreibung"/>
-    <tableColumn id="7" xr3:uid="{17A48F90-4A19-4F10-A7F2-C1A2D85DDBA7}" name="sensactIO4"/>
+    <tableColumn id="7" xr3:uid="{17A48F90-4A19-4F10-A7F2-C1A2D85DDBA7}" name="sensactHsNano"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -563,7 +527,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G2" sqref="G2:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +559,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -609,10 +573,7 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -625,9 +586,6 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -643,10 +601,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -660,10 +615,7 @@
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -673,9 +625,6 @@
       <c r="B6">
         <v>26</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -688,10 +637,7 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -795,10 +741,7 @@
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -811,9 +754,6 @@
       <c r="C15" t="s">
         <v>17</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -825,9 +765,6 @@
       <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -846,11 +783,9 @@
         <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -859,9 +794,6 @@
       <c r="B18">
         <v>27</v>
       </c>
-      <c r="G18">
-        <v>3</v>
-      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -870,9 +802,6 @@
       <c r="B19">
         <v>28</v>
       </c>
-      <c r="G19">
-        <v>4</v>
-      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -881,9 +810,6 @@
       <c r="B20">
         <v>30</v>
       </c>
-      <c r="G20">
-        <v>5</v>
-      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -892,9 +818,6 @@
       <c r="B21">
         <v>31</v>
       </c>
-      <c r="G21">
-        <v>6</v>
-      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -908,9 +831,6 @@
       <c r="B23">
         <v>33</v>
       </c>
-      <c r="G23" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -919,9 +839,6 @@
       <c r="B24">
         <v>36</v>
       </c>
-      <c r="G24" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -940,9 +857,6 @@
       <c r="B27">
         <v>10</v>
       </c>
-      <c r="G27">
-        <v>7</v>
-      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -951,9 +865,6 @@
       <c r="B28">
         <v>11</v>
       </c>
-      <c r="G28">
-        <v>8</v>
-      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -962,9 +873,6 @@
       <c r="B29">
         <v>12</v>
       </c>
-      <c r="G29">
-        <v>9</v>
-      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -976,9 +884,6 @@
       <c r="C30" t="s">
         <v>15</v>
       </c>
-      <c r="G30">
-        <v>10</v>
-      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -990,9 +895,6 @@
       <c r="C31" t="s">
         <v>14</v>
       </c>
-      <c r="G31">
-        <v>11</v>
-      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -1004,11 +906,8 @@
       <c r="D32" t="s">
         <v>13</v>
       </c>
-      <c r="G32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>35</v>
       </c>
@@ -1018,11 +917,8 @@
       <c r="D33" t="s">
         <v>13</v>
       </c>
-      <c r="G33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>36</v>
       </c>
@@ -1035,11 +931,8 @@
       <c r="D34" t="s">
         <v>13</v>
       </c>
-      <c r="G34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>39</v>
       </c>
@@ -1051,9 +944,6 @@
       </c>
       <c r="D35" t="s">
         <v>13</v>
-      </c>
-      <c r="G35" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>